<commit_message>
added fixations and separated stimulus array from probe
</commit_message>
<xml_diff>
--- a/html/resources/trials.xlsx
+++ b/html/resources/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/Desktop/change-localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9CBF45-5BB2-2845-B2C9-F0FF04D8E015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108E7695-E4BA-BE41-8C63-12DF841D7766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16700" xr2:uid="{784DD0E8-07A4-9C42-AB28-CAF75CA12E69}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>color1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>black</t>
   </si>
@@ -45,16 +42,28 @@
     <t>white</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>stim1</t>
-  </si>
-  <si>
-    <t>y_pos1</t>
-  </si>
-  <si>
-    <t>x_pos1</t>
+    <t>stim1_x</t>
+  </si>
+  <si>
+    <t>stim1_y</t>
+  </si>
+  <si>
+    <t>sitm1_color</t>
+  </si>
+  <si>
+    <t>probe1_x</t>
+  </si>
+  <si>
+    <t>probe1_y</t>
+  </si>
+  <si>
+    <t>probe1_color</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>probe1</t>
   </si>
 </sst>
 </file>
@@ -406,51 +415,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4529CD0-26AC-C541-BE97-9E8093EE6CB8}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="B2">
         <v>-0.25</v>
       </c>
       <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-0.25</v>
+      </c>
+      <c r="E2">
+        <v>-0.25</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>-0.25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extended stim durations and changed colors
</commit_message>
<xml_diff>
--- a/html/resources/trials.xlsx
+++ b/html/resources/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/Desktop/change-localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA678B7-BABA-724D-BAEA-1468BF13B0E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7A1A8-BBBC-8E4A-857E-7CD3364401A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13180" yWindow="460" windowWidth="14400" windowHeight="16700" xr2:uid="{784DD0E8-07A4-9C42-AB28-CAF75CA12E69}"/>
   </bookViews>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
     <t>stim1_x</t>
   </si>
   <si>
@@ -64,6 +58,12 @@
   </si>
   <si>
     <t>stim1_color</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blue</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,25 +428,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -457,7 +457,7 @@
         <v>-0.25</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>-0.25</v>
@@ -466,10 +466,10 @@
         <v>-0.25</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased set size to 2
</commit_message>
<xml_diff>
--- a/html/resources/trials.xlsx
+++ b/html/resources/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/Desktop/change-localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7A1A8-BBBC-8E4A-857E-7CD3364401A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A3CD5-2A22-9D4E-84E0-B16219B0FF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13180" yWindow="460" windowWidth="14400" windowHeight="16700" xr2:uid="{784DD0E8-07A4-9C42-AB28-CAF75CA12E69}"/>
   </bookViews>
@@ -34,29 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>stim1_x</t>
-  </si>
-  <si>
-    <t>stim1_y</t>
-  </si>
-  <si>
-    <t>probe1_x</t>
-  </si>
-  <si>
-    <t>probe1_y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>probe1_color</t>
   </si>
   <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>probe1</t>
-  </si>
-  <si>
     <t>stim1_color</t>
   </si>
   <si>
@@ -64,6 +46,30 @@
   </si>
   <si>
     <t>blue</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>stim2_color</t>
+  </si>
+  <si>
+    <t>probe2_color</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4529CD0-26AC-C541-BE97-9E8093EE6CB8}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,30 +432,33 @@
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-0.25</v>
       </c>
@@ -457,19 +466,48 @@
         <v>-0.25</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>-0.25</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
       </c>
       <c r="E2">
         <v>-0.25</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="F2">
+        <v>-0.25</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-0.25</v>
+      </c>
+      <c r="B3">
+        <v>-0.25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated positions and colors
</commit_message>
<xml_diff>
--- a/html/resources/trials.xlsx
+++ b/html/resources/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adkinsty/Desktop/change-localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A3CD5-2A22-9D4E-84E0-B16219B0FF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE3C654-9753-334F-B433-AF1394E88B91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13180" yWindow="460" windowWidth="14400" windowHeight="16700" xr2:uid="{784DD0E8-07A4-9C42-AB28-CAF75CA12E69}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,10 +460,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="B2">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -472,10 +472,10 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -486,10 +486,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="B3">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -498,10 +498,10 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>

</xml_diff>